<commit_message>
Real final version 4:30 am
</commit_message>
<xml_diff>
--- a/A2/Bertholin_destinvil-A2-correctionGrid.xlsx
+++ b/A2/Bertholin_destinvil-A2-correctionGrid.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="182">
   <si>
     <t>First Name</t>
   </si>
@@ -2122,8 +2122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV152"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A109" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B115" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5162,13 +5162,15 @@
         <v>127</v>
       </c>
       <c r="B123" s="22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C123" s="23"/>
       <c r="D123" s="12">
         <v>2</v>
       </c>
-      <c r="E123" s="29"/>
+      <c r="E123" s="29" t="s">
+        <v>181</v>
+      </c>
       <c r="F123" s="29"/>
       <c r="G123" s="7"/>
       <c r="H123" s="7"/>
@@ -5186,13 +5188,15 @@
         <v>128</v>
       </c>
       <c r="B124" s="22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C124" s="23"/>
       <c r="D124" s="12">
         <v>2</v>
       </c>
-      <c r="E124" s="29"/>
+      <c r="E124" s="29" t="s">
+        <v>181</v>
+      </c>
       <c r="F124" s="29"/>
       <c r="G124" s="7"/>
       <c r="H124" s="7"/>
@@ -5210,13 +5214,15 @@
         <v>129</v>
       </c>
       <c r="B125" s="22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C125" s="23"/>
       <c r="D125" s="12">
         <v>2</v>
       </c>
-      <c r="E125" s="29"/>
+      <c r="E125" s="29" t="s">
+        <v>181</v>
+      </c>
       <c r="F125" s="29"/>
       <c r="G125" s="7"/>
       <c r="H125" s="7"/>
@@ -5234,13 +5240,15 @@
         <v>130</v>
       </c>
       <c r="B126" s="22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C126" s="23"/>
       <c r="D126" s="12">
         <v>1</v>
       </c>
-      <c r="E126" s="29"/>
+      <c r="E126" s="29" t="s">
+        <v>181</v>
+      </c>
       <c r="F126" s="29"/>
       <c r="G126" s="7"/>
       <c r="H126" s="7"/>
@@ -5258,13 +5266,15 @@
         <v>131</v>
       </c>
       <c r="B127" s="22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C127" s="23"/>
       <c r="D127" s="12">
         <v>1</v>
       </c>
-      <c r="E127" s="29"/>
+      <c r="E127" s="29" t="s">
+        <v>181</v>
+      </c>
       <c r="F127" s="29"/>
       <c r="G127" s="7"/>
       <c r="H127" s="7"/>
@@ -5282,13 +5292,15 @@
         <v>132</v>
       </c>
       <c r="B128" s="22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C128" s="23"/>
       <c r="D128" s="12">
         <v>1</v>
       </c>
-      <c r="E128" s="29"/>
+      <c r="E128" s="29" t="s">
+        <v>181</v>
+      </c>
       <c r="F128" s="29"/>
       <c r="G128" s="7"/>
       <c r="H128" s="7"/>
@@ -5328,13 +5340,15 @@
         <v>134</v>
       </c>
       <c r="B130" s="22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C130" s="23"/>
       <c r="D130" s="12">
         <v>1</v>
       </c>
-      <c r="E130" s="29"/>
+      <c r="E130" s="29" t="s">
+        <v>181</v>
+      </c>
       <c r="F130" s="29"/>
       <c r="G130" s="7"/>
       <c r="H130" s="7"/>
@@ -5352,13 +5366,15 @@
         <v>135</v>
       </c>
       <c r="B131" s="22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C131" s="23"/>
       <c r="D131" s="12">
         <v>1</v>
       </c>
-      <c r="E131" s="29"/>
+      <c r="E131" s="29" t="s">
+        <v>181</v>
+      </c>
       <c r="F131" s="29"/>
       <c r="G131" s="7"/>
       <c r="H131" s="7"/>

</xml_diff>